<commit_message>
Ajout de notes précisant l'utilisation des données de la table principale uniquement et début de la préparation de ces données
</commit_message>
<xml_diff>
--- a/code/data/brutes/HomeCredit_columns_description.xlsx
+++ b/code/data/brutes/HomeCredit_columns_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbourgeois\Desktop\OC\oc-p7-implementer-modele-scoring\code\data\brutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B22272E-206B-4B45-9F2D-3FE2905F12EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FDE52E-306A-4F21-B599-1882C597D4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D34379C3-A7DB-48BB-AE29-5E68E882D796}"/>
   </bookViews>
@@ -1276,7 +1276,12 @@
   <autoFilter ref="A1:F220" xr:uid="{58CF4FF9-B3DD-4B76-B940-AEBB2973D6A0}">
     <filterColumn colId="1">
       <filters>
-        <filter val="bureau.csv"/>
+        <filter val="application_{train|test}.csv"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1285,8 +1290,8 @@
     <tableColumn id="2" xr3:uid="{E0774EC9-5C77-40E3-A058-056CF6B5E7A3}" uniqueName="2" name="Table" queryTableFieldId="2" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{49337099-C203-4C1B-B37B-0FE990558EDF}" uniqueName="3" name="Row" queryTableFieldId="3" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{46AE20F0-B2C0-4C6A-9A43-BDA36F7310A6}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{30B5F825-44D4-4AF9-8A71-D3CD1397934A}" uniqueName="6" name="To be kept" queryTableFieldId="6" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{E3D20E3A-CA3A-491A-8A82-0B81C7F83DD1}" uniqueName="5" name="Special" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{30B5F825-44D4-4AF9-8A71-D3CD1397934A}" uniqueName="6" name="To be kept" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{E3D20E3A-CA3A-491A-8A82-0B81C7F83DD1}" uniqueName="5" name="Special" queryTableFieldId="5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1592,7 +1597,7 @@
   <dimension ref="A1:F220"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134"/>
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1624,7 +1629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1644,7 +1649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1664,7 +1669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1684,7 +1689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1704,7 +1709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>7</v>
       </c>
@@ -1724,7 +1729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>8</v>
       </c>
@@ -1744,7 +1749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1764,7 +1769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>10</v>
       </c>
@@ -1784,7 +1789,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>11</v>
       </c>
@@ -1804,7 +1809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>12</v>
       </c>
@@ -1824,7 +1829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>13</v>
       </c>
@@ -1864,7 +1869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>15</v>
       </c>
@@ -1904,7 +1909,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>17</v>
       </c>
@@ -1924,7 +1929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>18</v>
       </c>
@@ -1964,7 +1969,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>20</v>
       </c>
@@ -1984,7 +1989,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>21</v>
       </c>
@@ -2044,7 +2049,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>24</v>
       </c>
@@ -2184,7 +2189,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>31</v>
       </c>
@@ -2204,7 +2209,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>32</v>
       </c>
@@ -2424,7 +2429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>43</v>
       </c>
@@ -3444,7 +3449,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>94</v>
       </c>
@@ -3464,7 +3469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>95</v>
       </c>
@@ -3484,7 +3489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>96</v>
       </c>
@@ -3504,7 +3509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>97</v>
       </c>
@@ -4064,7 +4069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>125</v>
       </c>
@@ -4084,7 +4089,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>126</v>
       </c>
@@ -4104,7 +4109,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>127</v>
       </c>
@@ -4124,7 +4129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>128</v>
       </c>
@@ -4144,7 +4149,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>129</v>
       </c>
@@ -4164,7 +4169,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>130</v>
       </c>
@@ -4184,7 +4189,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>131</v>
       </c>
@@ -4204,7 +4209,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>132</v>
       </c>
@@ -4224,7 +4229,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>133</v>
       </c>
@@ -4244,7 +4249,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>134</v>
       </c>
@@ -4264,7 +4269,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>135</v>
       </c>
@@ -4284,7 +4289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>136</v>
       </c>
@@ -4304,7 +4309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>137</v>
       </c>
@@ -4324,7 +4329,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>138</v>
       </c>
@@ -4344,7 +4349,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>139</v>
       </c>
@@ -4364,7 +4369,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>140</v>
       </c>
@@ -4384,7 +4389,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>141</v>
       </c>

</xml_diff>

<commit_message>
Suppression de la variable 'ORGANIZATION_TYPE' et ajout de 'NAME_EDUCATION_TYPE'
</commit_message>
<xml_diff>
--- a/code/data/brutes/HomeCredit_columns_description.xlsx
+++ b/code/data/brutes/HomeCredit_columns_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbourgeois\Desktop\OC\oc-p7-implementer-modele-scoring\code\data\brutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FDE52E-306A-4F21-B599-1882C597D4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75056496-2FA9-4B39-B5C6-9F95B5DE238B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D34379C3-A7DB-48BB-AE29-5E68E882D796}"/>
   </bookViews>
@@ -1597,7 +1597,7 @@
   <dimension ref="A1:F220"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1889,7 +1889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>16</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>34</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>8</v>

</xml_diff>